<commit_message>
colocando seção para baixar musica
</commit_message>
<xml_diff>
--- a/data/download_list.xlsx
+++ b/data/download_list.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\youtube_downloader\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6329E4-2914-4AA6-BB4E-D77E39C6A37E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92E24AD-C29A-4AF9-A56D-ACBCB1EC78A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lives" sheetId="1" r:id="rId1"/>
-    <sheet name="videos" sheetId="2" r:id="rId2"/>
+    <sheet name="musicas_de_sogro" sheetId="3" r:id="rId2"/>
+    <sheet name="videos" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t>name</t>
   </si>
@@ -79,7 +80,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -385,7 +386,7 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -416,6 +417,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9B7C2A7-03F4-4CFB-B588-25B438F8F2C8}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>

</xml_diff>